<commit_message>
Update all templates to follow same style
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_4.xlsx
+++ b/templates/NHWA_Module_4.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20350"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\EyeSeeTea\excel-data-import-app\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\EST\Excel_Data_Importer\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="kJpbPdv3VXwiW4mW24e4Dcs7ERib884M9ASxhUSAaPZWg8QdDkhdrbzpLspRzLvDk3+kcuxNboiZ4Yurmbs8+w==" workbookSaltValue="o1Q3IOmNfHgUyE6fE82NdA==" workbookSpinCount="100000" lockStructure="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1930F3A9-2EC9-4384-8C97-F581C1DA93F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="haj4Cbed6/r1AwHDnh+HLyke+LyqX3ZWhaY7c6jINshTd1o4RMDFEE9LnRDo6lfAHDnbOy9lJvibL3SZsRqM6g==" workbookSaltValue="zFLirmJ+0Pgso8hCRJ/84w==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="391"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14100" tabRatio="391" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Finance" sheetId="1" r:id="rId1"/>
@@ -21,12 +22,12 @@
   <definedNames>
     <definedName name="dropdownlist">Finance!$AE$2:INDEX(Finance!$AE$2:$AE$250,MAX(Finance!$AD$2:$AD$250),1)</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="802">
   <si>
     <t xml:space="preserve">NATIONAL  HEALTH WORKFORCE ACCOUNTS DATA </t>
   </si>
@@ -2433,12 +2434,15 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>Total Cost per graduate in medical specialist education programmes (4-06)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -2532,7 +2536,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -2595,15 +2599,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -2611,26 +2606,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -2645,17 +2620,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -2675,17 +2639,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -2715,7 +2668,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2770,20 +2723,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2814,30 +2758,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2845,30 +2779,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2888,75 +2798,70 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
-    <cellStyle name="40% - Énfasis1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma [0] 2" xfId="3"/>
-    <cellStyle name="Comma [0] 3" xfId="4"/>
-    <cellStyle name="Comma 2" xfId="5"/>
-    <cellStyle name="Comma 3" xfId="6"/>
-    <cellStyle name="Comma 4" xfId="7"/>
-    <cellStyle name="Comma 5" xfId="2"/>
-    <cellStyle name="flashing" xfId="8"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma [0] 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Comma [0] 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Comma 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Comma 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Comma 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Comma 5" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="flashing" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="9"/>
-    <cellStyle name="Normal 3" xfId="10"/>
-    <cellStyle name="Normal 3 2" xfId="11"/>
-    <cellStyle name="Normal 4" xfId="12"/>
-    <cellStyle name="Normal 4 2" xfId="13"/>
-    <cellStyle name="Normal 5" xfId="14"/>
-    <cellStyle name="Normal 6" xfId="15"/>
-    <cellStyle name="Normal 7" xfId="16"/>
-    <cellStyle name="Normal 8" xfId="17"/>
-    <cellStyle name="tgl" xfId="18"/>
+    <cellStyle name="Normal 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 3" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 3 2" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 4" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 4 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 5" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 6" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 7" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal 8" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="tgl" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2986,13 +2891,13 @@
       <xdr:twoCellAnchor>
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>713014</xdr:colOff>
+          <xdr:colOff>714375</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>277586</xdr:rowOff>
+          <xdr:rowOff>276225</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>10886</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -3044,15 +2949,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>620486</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>14</xdr:row>
-          <xdr:rowOff>179614</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>963386</xdr:colOff>
-          <xdr:row>14</xdr:row>
-          <xdr:rowOff>478971</xdr:rowOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3101,7 +3006,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3176,6 +3081,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3211,6 +3133,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3386,50 +3325,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BZ250"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15:E15"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.15234375" style="4"/>
-    <col min="2" max="2" width="10.84375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="76.69140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.84375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="21.53515625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="21.921875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="18.69140625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="15.53515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="76.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="21.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" style="4" customWidth="1"/>
     <col min="9" max="9" width="16" style="4" customWidth="1"/>
-    <col min="10" max="10" width="10.3046875" style="4" customWidth="1"/>
-    <col min="11" max="15" width="9.15234375" style="4" customWidth="1"/>
-    <col min="16" max="16" width="12.53515625" style="4" customWidth="1"/>
-    <col min="17" max="17" width="11.53515625" style="4" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="16.3046875" style="4" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="4" customWidth="1"/>
+    <col min="11" max="15" width="9.140625" style="4" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" style="4" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="16.28515625" style="4" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="12" style="4" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="12.15234375" style="4" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="9.69140625" style="4" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="16.84375" style="4" hidden="1" customWidth="1"/>
-    <col min="23" max="33" width="9.15234375" style="4" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="12.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="16.85546875" style="4" hidden="1" customWidth="1"/>
+    <col min="23" max="33" width="9.140625" style="4" hidden="1" customWidth="1"/>
     <col min="34" max="34" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.15234375" style="4"/>
+    <col min="35" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:31" ht="22.75" x14ac:dyDescent="0.4">
-      <c r="B1" s="44" t="s">
+    <row r="1" spans="2:31" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -3459,17 +3398,17 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="2:31" ht="22.75" x14ac:dyDescent="0.4">
-      <c r="B2" s="44" t="s">
+    <row r="2" spans="2:31" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B2" s="39" t="s">
         <v>775</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -3512,7 +3451,7 @@
         <v>Algeria</v>
       </c>
     </row>
-    <row r="3" spans="2:31" ht="22.75" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:31" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -3522,17 +3461,17 @@
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
-      <c r="U3" s="26"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
       <c r="V3" s="11"/>
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
@@ -3561,21 +3500,21 @@
         <v>Angola</v>
       </c>
     </row>
-    <row r="4" spans="2:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:31" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="35" t="str">
+      <c r="E4" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="32" t="str">
         <f>IFERROR(VLOOKUP(V1,Y2:AB250,4,0),"")</f>
         <v/>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="34"/>
+      <c r="I4" s="31"/>
       <c r="Y4" s="4" t="s">
         <v>12</v>
       </c>
@@ -3601,7 +3540,7 @@
         <v>Benin</v>
       </c>
     </row>
-    <row r="5" spans="2:31" ht="22.75" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18"/>
       <c r="C5" s="18"/>
       <c r="D5" s="2"/>
@@ -3644,8 +3583,8 @@
         <v>Botswana</v>
       </c>
     </row>
-    <row r="6" spans="2:31" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="B6" s="23"/>
+    <row r="6" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="21"/>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
@@ -3685,25 +3624,25 @@
         <v>Burkina Faso</v>
       </c>
     </row>
-    <row r="7" spans="2:31" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="B7" s="39" t="s">
+    <row r="7" spans="2:31" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="38" t="s">
         <v>765</v>
       </c>
-      <c r="D7" s="45" t="s">
+      <c r="D7" s="40" t="s">
         <v>766</v>
       </c>
-      <c r="E7" s="45" t="s">
+      <c r="E7" s="40" t="s">
         <v>762</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
       <c r="R7" s="13"/>
@@ -3734,17 +3673,17 @@
         <v>Burundi</v>
       </c>
     </row>
-    <row r="8" spans="2:31" ht="47.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="24" t="s">
+    <row r="8" spans="2:31" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="22" t="s">
         <v>767</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="22" t="s">
         <v>768</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="22" t="s">
         <v>769</v>
       </c>
       <c r="H8" s="20"/>
@@ -3781,17 +3720,17 @@
         <v>Cabo Verde</v>
       </c>
     </row>
-    <row r="9" spans="2:31" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="21">
-        <v>1</v>
-      </c>
-      <c r="C9" s="74" t="s">
+    <row r="9" spans="2:31" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="51">
+        <v>1</v>
+      </c>
+      <c r="C9" s="49" t="s">
         <v>773</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
       <c r="N9" s="14"/>
@@ -3826,17 +3765,17 @@
         <v>Cameroon</v>
       </c>
     </row>
-    <row r="10" spans="2:31" ht="19" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="25">
+    <row r="10" spans="2:31" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="35">
         <v>2</v>
       </c>
-      <c r="C10" s="74" t="s">
+      <c r="C10" s="34" t="s">
         <v>798</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
       <c r="N10" s="14"/>
@@ -3871,13 +3810,13 @@
         <v>Central African Republic</v>
       </c>
     </row>
-    <row r="11" spans="2:31" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="B11" s="52"/>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
+    <row r="11" spans="2:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
       <c r="N11" s="14"/>
@@ -3912,13 +3851,13 @@
         <v>Chad</v>
       </c>
     </row>
-    <row r="12" spans="2:31" ht="15.9" x14ac:dyDescent="0.45">
-      <c r="B12" s="52"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="52"/>
-      <c r="E12" s="52"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
+    <row r="12" spans="2:31" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
       <c r="N12" s="14"/>
@@ -3953,21 +3892,21 @@
         <v>Comoros</v>
       </c>
     </row>
-    <row r="13" spans="2:31" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="38" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="38" t="s">
         <v>765</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="38" t="s">
         <v>799</v>
       </c>
-      <c r="E13" s="47"/>
-      <c r="F13" s="46" t="s">
+      <c r="E13" s="38"/>
+      <c r="F13" s="38" t="s">
         <v>800</v>
       </c>
-      <c r="G13" s="50"/>
+      <c r="G13" s="38"/>
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
@@ -3996,13 +3935,13 @@
         <v>Congo</v>
       </c>
     </row>
-    <row r="14" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="51"/>
+    <row r="14" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
       <c r="N14" s="14"/>
       <c r="O14" s="14"/>
       <c r="P14" s="14"/>
@@ -4034,17 +3973,17 @@
         <v>Cote d'Ivoire</v>
       </c>
     </row>
-    <row r="15" spans="2:31" ht="47.6" x14ac:dyDescent="0.45">
-      <c r="B15" s="21">
-        <v>1</v>
-      </c>
-      <c r="C15" s="75" t="s">
+    <row r="15" spans="2:31" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B15" s="52">
+        <v>1</v>
+      </c>
+      <c r="C15" s="53" t="s">
         <v>774</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="43"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="59"/>
       <c r="N15" s="14"/>
       <c r="O15" s="14"/>
       <c r="P15" s="14"/>
@@ -4076,7 +4015,7 @@
         <v>Democratic Republic of the Congo</v>
       </c>
     </row>
-    <row r="16" spans="2:31" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
       <c r="V16" s="4" t="s">
         <v>764</v>
       </c>
@@ -4105,7 +4044,7 @@
         <v>Equatorial Guinea</v>
       </c>
     </row>
-    <row r="17" spans="6:31" x14ac:dyDescent="0.4">
+    <row r="17" spans="6:31" x14ac:dyDescent="0.25">
       <c r="Q17" s="4" t="s">
         <v>763</v>
       </c>
@@ -4143,8 +4082,8 @@
         <v>Eritrea</v>
       </c>
     </row>
-    <row r="18" spans="6:31" x14ac:dyDescent="0.4">
-      <c r="F18" s="36"/>
+    <row r="18" spans="6:31" x14ac:dyDescent="0.25">
+      <c r="F18" s="33"/>
       <c r="Q18" s="4" t="str">
         <f>IF(V17=2,"True","")</f>
         <v/>
@@ -4182,7 +4121,7 @@
         <v>Ethiopia</v>
       </c>
     </row>
-    <row r="19" spans="6:31" x14ac:dyDescent="0.4">
+    <row r="19" spans="6:31" x14ac:dyDescent="0.25">
       <c r="Y19" s="4" t="s">
         <v>24</v>
       </c>
@@ -4208,7 +4147,7 @@
         <v>Gabon</v>
       </c>
     </row>
-    <row r="20" spans="6:31" ht="15" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="6:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Y20" s="4" t="s">
         <v>25</v>
       </c>
@@ -4234,7 +4173,7 @@
         <v>Gambia</v>
       </c>
     </row>
-    <row r="21" spans="6:31" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="6:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Y21" s="4" t="s">
         <v>26</v>
       </c>
@@ -4260,7 +4199,7 @@
         <v>Ghana</v>
       </c>
     </row>
-    <row r="22" spans="6:31" ht="35.700000000000003" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="6:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Y22" s="4" t="s">
         <v>27</v>
       </c>
@@ -4286,7 +4225,7 @@
         <v>Guinea</v>
       </c>
     </row>
-    <row r="23" spans="6:31" x14ac:dyDescent="0.4">
+    <row r="23" spans="6:31" x14ac:dyDescent="0.25">
       <c r="Y23" s="4" t="s">
         <v>28</v>
       </c>
@@ -4312,7 +4251,7 @@
         <v>Guinea-Bissau</v>
       </c>
     </row>
-    <row r="24" spans="6:31" x14ac:dyDescent="0.4">
+    <row r="24" spans="6:31" x14ac:dyDescent="0.25">
       <c r="Y24" s="4" t="s">
         <v>29</v>
       </c>
@@ -4338,7 +4277,7 @@
         <v>Kenya</v>
       </c>
     </row>
-    <row r="25" spans="6:31" x14ac:dyDescent="0.4">
+    <row r="25" spans="6:31" x14ac:dyDescent="0.25">
       <c r="Y25" s="4" t="s">
         <v>30</v>
       </c>
@@ -4364,7 +4303,7 @@
         <v>Lesotho</v>
       </c>
     </row>
-    <row r="26" spans="6:31" x14ac:dyDescent="0.4">
+    <row r="26" spans="6:31" x14ac:dyDescent="0.25">
       <c r="Y26" s="4" t="s">
         <v>31</v>
       </c>
@@ -4390,7 +4329,7 @@
         <v>Liberia</v>
       </c>
     </row>
-    <row r="27" spans="6:31" x14ac:dyDescent="0.4">
+    <row r="27" spans="6:31" x14ac:dyDescent="0.25">
       <c r="Y27" s="4" t="s">
         <v>32</v>
       </c>
@@ -4416,7 +4355,7 @@
         <v>Madagascar</v>
       </c>
     </row>
-    <row r="28" spans="6:31" x14ac:dyDescent="0.4">
+    <row r="28" spans="6:31" x14ac:dyDescent="0.25">
       <c r="Y28" s="4" t="s">
         <v>33</v>
       </c>
@@ -4442,7 +4381,7 @@
         <v>Malawi</v>
       </c>
     </row>
-    <row r="29" spans="6:31" x14ac:dyDescent="0.4">
+    <row r="29" spans="6:31" x14ac:dyDescent="0.25">
       <c r="Y29" s="4" t="s">
         <v>34</v>
       </c>
@@ -4468,7 +4407,7 @@
         <v>Mali</v>
       </c>
     </row>
-    <row r="30" spans="6:31" x14ac:dyDescent="0.4">
+    <row r="30" spans="6:31" x14ac:dyDescent="0.25">
       <c r="Y30" s="4" t="s">
         <v>35</v>
       </c>
@@ -4494,7 +4433,7 @@
         <v>Mauritania</v>
       </c>
     </row>
-    <row r="31" spans="6:31" x14ac:dyDescent="0.4">
+    <row r="31" spans="6:31" x14ac:dyDescent="0.25">
       <c r="Y31" s="4" t="s">
         <v>36</v>
       </c>
@@ -4520,7 +4459,7 @@
         <v>Mauritius</v>
       </c>
     </row>
-    <row r="32" spans="6:31" x14ac:dyDescent="0.4">
+    <row r="32" spans="6:31" x14ac:dyDescent="0.25">
       <c r="Y32" s="4" t="s">
         <v>37</v>
       </c>
@@ -4546,7 +4485,7 @@
         <v>Mozambique</v>
       </c>
     </row>
-    <row r="33" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="33" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y33" s="4" t="s">
         <v>38</v>
       </c>
@@ -4572,7 +4511,7 @@
         <v>Namibia</v>
       </c>
     </row>
-    <row r="34" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="34" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y34" s="4" t="s">
         <v>39</v>
       </c>
@@ -4598,7 +4537,7 @@
         <v>Niger</v>
       </c>
     </row>
-    <row r="35" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="35" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y35" s="4" t="s">
         <v>40</v>
       </c>
@@ -4624,7 +4563,7 @@
         <v>Nigeria</v>
       </c>
     </row>
-    <row r="36" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="36" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y36" s="4" t="s">
         <v>41</v>
       </c>
@@ -4650,7 +4589,7 @@
         <v>Rwanda</v>
       </c>
     </row>
-    <row r="37" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="37" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y37" s="4" t="s">
         <v>42</v>
       </c>
@@ -4676,7 +4615,7 @@
         <v>Sao Tome and Principe</v>
       </c>
     </row>
-    <row r="38" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="38" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y38" s="4" t="s">
         <v>43</v>
       </c>
@@ -4702,7 +4641,7 @@
         <v>Senegal</v>
       </c>
     </row>
-    <row r="39" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="39" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y39" s="4" t="s">
         <v>44</v>
       </c>
@@ -4728,7 +4667,7 @@
         <v>Seychelles</v>
       </c>
     </row>
-    <row r="40" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="40" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y40" s="4" t="s">
         <v>45</v>
       </c>
@@ -4754,7 +4693,7 @@
         <v>Sierra Leone</v>
       </c>
     </row>
-    <row r="41" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="41" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y41" s="4" t="s">
         <v>46</v>
       </c>
@@ -4780,7 +4719,7 @@
         <v>South Africa</v>
       </c>
     </row>
-    <row r="42" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="42" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y42" s="4" t="s">
         <v>282</v>
       </c>
@@ -4806,7 +4745,7 @@
         <v>South Sudan</v>
       </c>
     </row>
-    <row r="43" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="43" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y43" s="4" t="s">
         <v>47</v>
       </c>
@@ -4832,7 +4771,7 @@
         <v>Swaziland</v>
       </c>
     </row>
-    <row r="44" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="44" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y44" s="4" t="s">
         <v>48</v>
       </c>
@@ -4858,7 +4797,7 @@
         <v>Togo</v>
       </c>
     </row>
-    <row r="45" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="45" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y45" s="4" t="s">
         <v>49</v>
       </c>
@@ -4884,7 +4823,7 @@
         <v>Uganda</v>
       </c>
     </row>
-    <row r="46" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="46" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y46" s="4" t="s">
         <v>50</v>
       </c>
@@ -4910,7 +4849,7 @@
         <v>United Republic of Tanzania</v>
       </c>
     </row>
-    <row r="47" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="47" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y47" s="4" t="s">
         <v>51</v>
       </c>
@@ -4936,7 +4875,7 @@
         <v>Zambia</v>
       </c>
     </row>
-    <row r="48" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="48" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y48" s="4" t="s">
         <v>52</v>
       </c>
@@ -4962,7 +4901,7 @@
         <v>Zimbabwe</v>
       </c>
     </row>
-    <row r="49" spans="1:78" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:78" x14ac:dyDescent="0.25">
       <c r="Y49" s="4" t="s">
         <v>53</v>
       </c>
@@ -4988,7 +4927,7 @@
         <v>Antigua and Barbuda</v>
       </c>
     </row>
-    <row r="50" spans="1:78" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:78" x14ac:dyDescent="0.25">
       <c r="Y50" s="4" t="s">
         <v>54</v>
       </c>
@@ -5014,7 +4953,7 @@
         <v>Argentina</v>
       </c>
     </row>
-    <row r="51" spans="1:78" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:78" x14ac:dyDescent="0.25">
       <c r="Y51" s="4" t="s">
         <v>302</v>
       </c>
@@ -5040,7 +4979,7 @@
         <v>Bahamas</v>
       </c>
     </row>
-    <row r="52" spans="1:78" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:78" x14ac:dyDescent="0.25">
       <c r="Y52" s="4" t="s">
         <v>55</v>
       </c>
@@ -5066,7 +5005,7 @@
         <v>Barbados</v>
       </c>
     </row>
-    <row r="53" spans="1:78" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:78" x14ac:dyDescent="0.25">
       <c r="Y53" s="4" t="s">
         <v>56</v>
       </c>
@@ -5092,7 +5031,7 @@
         <v>Belize</v>
       </c>
     </row>
-    <row r="54" spans="1:78" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:78" x14ac:dyDescent="0.25">
       <c r="Y54" s="4" t="s">
         <v>57</v>
       </c>
@@ -5118,7 +5057,7 @@
         <v>Bolivia (Plurinational State of)</v>
       </c>
     </row>
-    <row r="57" spans="1:78" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:78" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -5215,7 +5154,7 @@
       <c r="BY57" s="4"/>
       <c r="BZ57" s="4"/>
     </row>
-    <row r="58" spans="1:78" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:78" x14ac:dyDescent="0.25">
       <c r="Y58" s="4" t="s">
         <v>59</v>
       </c>
@@ -5241,7 +5180,7 @@
         <v>Colombia</v>
       </c>
     </row>
-    <row r="59" spans="1:78" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:78" x14ac:dyDescent="0.25">
       <c r="Y59" s="4" t="s">
         <v>60</v>
       </c>
@@ -5267,7 +5206,7 @@
         <v>Costa Rica</v>
       </c>
     </row>
-    <row r="60" spans="1:78" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:78" x14ac:dyDescent="0.25">
       <c r="Y60" s="4" t="s">
         <v>61</v>
       </c>
@@ -5293,7 +5232,7 @@
         <v>Cuba</v>
       </c>
     </row>
-    <row r="61" spans="1:78" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:78" x14ac:dyDescent="0.25">
       <c r="Y61" s="4" t="s">
         <v>62</v>
       </c>
@@ -5319,7 +5258,7 @@
         <v>Dominica</v>
       </c>
     </row>
-    <row r="62" spans="1:78" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:78" x14ac:dyDescent="0.25">
       <c r="Y62" s="4" t="s">
         <v>63</v>
       </c>
@@ -5345,7 +5284,7 @@
         <v>Dominican Republic</v>
       </c>
     </row>
-    <row r="63" spans="1:78" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:78" x14ac:dyDescent="0.25">
       <c r="Y63" s="4" t="s">
         <v>64</v>
       </c>
@@ -5371,7 +5310,7 @@
         <v>Ecuador</v>
       </c>
     </row>
-    <row r="64" spans="1:78" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:78" x14ac:dyDescent="0.25">
       <c r="Y64" s="4" t="s">
         <v>65</v>
       </c>
@@ -5397,7 +5336,7 @@
         <v>El Salvador</v>
       </c>
     </row>
-    <row r="65" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="65" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y65" s="4" t="s">
         <v>66</v>
       </c>
@@ -5423,7 +5362,7 @@
         <v>Grenada</v>
       </c>
     </row>
-    <row r="66" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="66" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y66" s="4" t="s">
         <v>67</v>
       </c>
@@ -5449,7 +5388,7 @@
         <v>Guatemala</v>
       </c>
     </row>
-    <row r="67" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="67" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y67" s="4" t="s">
         <v>68</v>
       </c>
@@ -5475,7 +5414,7 @@
         <v>Guyana</v>
       </c>
     </row>
-    <row r="68" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="68" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y68" s="4" t="s">
         <v>69</v>
       </c>
@@ -5501,7 +5440,7 @@
         <v>Haiti</v>
       </c>
     </row>
-    <row r="69" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="69" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y69" s="4" t="s">
         <v>70</v>
       </c>
@@ -5527,7 +5466,7 @@
         <v>Honduras</v>
       </c>
     </row>
-    <row r="70" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="70" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y70" s="4" t="s">
         <v>71</v>
       </c>
@@ -5553,7 +5492,7 @@
         <v>Jamaica</v>
       </c>
     </row>
-    <row r="71" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="71" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y71" s="4" t="s">
         <v>72</v>
       </c>
@@ -5579,7 +5518,7 @@
         <v>Mexico</v>
       </c>
     </row>
-    <row r="72" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="72" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y72" s="4" t="s">
         <v>73</v>
       </c>
@@ -5605,7 +5544,7 @@
         <v>Nicaragua</v>
       </c>
     </row>
-    <row r="73" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="73" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y73" s="4" t="s">
         <v>74</v>
       </c>
@@ -5631,7 +5570,7 @@
         <v>Panama</v>
       </c>
     </row>
-    <row r="74" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="74" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y74" s="4" t="s">
         <v>75</v>
       </c>
@@ -5657,7 +5596,7 @@
         <v>Paraguay</v>
       </c>
     </row>
-    <row r="75" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="75" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y75" s="4" t="s">
         <v>76</v>
       </c>
@@ -5683,7 +5622,7 @@
         <v>Peru</v>
       </c>
     </row>
-    <row r="76" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="76" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y76" s="4" t="s">
         <v>77</v>
       </c>
@@ -5709,7 +5648,7 @@
         <v>Saint Kitts and Nevis</v>
       </c>
     </row>
-    <row r="77" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="77" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y77" s="4" t="s">
         <v>78</v>
       </c>
@@ -5735,7 +5674,7 @@
         <v>Saint Lucia</v>
       </c>
     </row>
-    <row r="78" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="78" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y78" s="4" t="s">
         <v>79</v>
       </c>
@@ -5761,7 +5700,7 @@
         <v>Saint Vincent and the Grenadines</v>
       </c>
     </row>
-    <row r="79" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="79" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y79" s="4" t="s">
         <v>80</v>
       </c>
@@ -5787,7 +5726,7 @@
         <v>Suriname</v>
       </c>
     </row>
-    <row r="80" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="80" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y80" s="4" t="s">
         <v>81</v>
       </c>
@@ -5813,7 +5752,7 @@
         <v>Trinidad and Tobago</v>
       </c>
     </row>
-    <row r="81" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="81" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y81" s="4" t="s">
         <v>82</v>
       </c>
@@ -5839,7 +5778,7 @@
         <v>United States of America</v>
       </c>
     </row>
-    <row r="82" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="82" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y82" s="4" t="s">
         <v>83</v>
       </c>
@@ -5865,7 +5804,7 @@
         <v>Uruguay</v>
       </c>
     </row>
-    <row r="83" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="83" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y83" s="4" t="s">
         <v>84</v>
       </c>
@@ -5891,7 +5830,7 @@
         <v>Venezuela (Bolivarian Republic of)</v>
       </c>
     </row>
-    <row r="84" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="84" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y84" s="4" t="s">
         <v>85</v>
       </c>
@@ -5917,7 +5856,7 @@
         <v>Afghanistan</v>
       </c>
     </row>
-    <row r="85" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="85" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y85" s="4" t="s">
         <v>86</v>
       </c>
@@ -5943,7 +5882,7 @@
         <v>Bahrain</v>
       </c>
     </row>
-    <row r="86" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="86" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y86" s="4" t="s">
         <v>87</v>
       </c>
@@ -5969,7 +5908,7 @@
         <v>Djibouti</v>
       </c>
     </row>
-    <row r="87" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="87" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y87" s="4" t="s">
         <v>88</v>
       </c>
@@ -5995,7 +5934,7 @@
         <v>Egypt</v>
       </c>
     </row>
-    <row r="88" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="88" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y88" s="4" t="s">
         <v>89</v>
       </c>
@@ -6021,7 +5960,7 @@
         <v>Iran (Islamic Republic of)</v>
       </c>
     </row>
-    <row r="89" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="89" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y89" s="4" t="s">
         <v>90</v>
       </c>
@@ -6047,7 +5986,7 @@
         <v>Iraq</v>
       </c>
     </row>
-    <row r="90" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="90" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y90" s="4" t="s">
         <v>91</v>
       </c>
@@ -6073,7 +6012,7 @@
         <v>Jordan</v>
       </c>
     </row>
-    <row r="91" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="91" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y91" s="4" t="s">
         <v>92</v>
       </c>
@@ -6099,7 +6038,7 @@
         <v>Kuwait</v>
       </c>
     </row>
-    <row r="92" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="92" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y92" s="4" t="s">
         <v>93</v>
       </c>
@@ -6125,7 +6064,7 @@
         <v>Lebanon</v>
       </c>
     </row>
-    <row r="93" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="93" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y93" s="4" t="s">
         <v>94</v>
       </c>
@@ -6151,7 +6090,7 @@
         <v>Libya</v>
       </c>
     </row>
-    <row r="94" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="94" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y94" s="4" t="s">
         <v>95</v>
       </c>
@@ -6177,7 +6116,7 @@
         <v>Morocco</v>
       </c>
     </row>
-    <row r="95" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="95" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y95" s="4" t="s">
         <v>388</v>
       </c>
@@ -6203,7 +6142,7 @@
         <v>Oman</v>
       </c>
     </row>
-    <row r="96" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="96" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y96" s="4" t="s">
         <v>96</v>
       </c>
@@ -6229,7 +6168,7 @@
         <v>Pakistan</v>
       </c>
     </row>
-    <row r="97" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="97" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y97" s="4" t="s">
         <v>97</v>
       </c>
@@ -6255,7 +6194,7 @@
         <v>Palestine</v>
       </c>
     </row>
-    <row r="98" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="98" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y98" s="4" t="s">
         <v>98</v>
       </c>
@@ -6281,7 +6220,7 @@
         <v>Qatar</v>
       </c>
     </row>
-    <row r="99" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="99" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y99" s="4" t="s">
         <v>397</v>
       </c>
@@ -6307,7 +6246,7 @@
         <v>Saudi Arabia</v>
       </c>
     </row>
-    <row r="100" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="100" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y100" s="4" t="s">
         <v>99</v>
       </c>
@@ -6333,7 +6272,7 @@
         <v>Somalia</v>
       </c>
     </row>
-    <row r="101" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="101" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y101" s="4" t="s">
         <v>100</v>
       </c>
@@ -6359,7 +6298,7 @@
         <v>Sudan</v>
       </c>
     </row>
-    <row r="102" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="102" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y102" s="4" t="s">
         <v>101</v>
       </c>
@@ -6385,7 +6324,7 @@
         <v>Syrian Arab Republic</v>
       </c>
     </row>
-    <row r="103" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="103" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y103" s="4" t="s">
         <v>102</v>
       </c>
@@ -6411,7 +6350,7 @@
         <v>Tunisia</v>
       </c>
     </row>
-    <row r="104" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="104" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y104" s="4" t="s">
         <v>103</v>
       </c>
@@ -6437,7 +6376,7 @@
         <v>United Arab Emirates</v>
       </c>
     </row>
-    <row r="105" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="105" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y105" s="4" t="s">
         <v>104</v>
       </c>
@@ -6463,7 +6402,7 @@
         <v>Yemen</v>
       </c>
     </row>
-    <row r="106" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="106" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y106" s="4" t="s">
         <v>105</v>
       </c>
@@ -6489,7 +6428,7 @@
         <v>Albania</v>
       </c>
     </row>
-    <row r="107" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="107" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y107" s="4" t="s">
         <v>106</v>
       </c>
@@ -6515,7 +6454,7 @@
         <v>Andorra</v>
       </c>
     </row>
-    <row r="108" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="108" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y108" s="4" t="s">
         <v>107</v>
       </c>
@@ -6541,7 +6480,7 @@
         <v>Armenia</v>
       </c>
     </row>
-    <row r="109" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="109" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y109" s="4" t="s">
         <v>108</v>
       </c>
@@ -6567,7 +6506,7 @@
         <v>Austria</v>
       </c>
     </row>
-    <row r="110" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="110" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y110" s="4" t="s">
         <v>109</v>
       </c>
@@ -6593,7 +6532,7 @@
         <v>Azerbaijan</v>
       </c>
     </row>
-    <row r="111" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="111" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y111" s="4" t="s">
         <v>110</v>
       </c>
@@ -6619,7 +6558,7 @@
         <v>Belarus</v>
       </c>
     </row>
-    <row r="112" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="112" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y112" s="4" t="s">
         <v>111</v>
       </c>
@@ -6645,7 +6584,7 @@
         <v>Belgium</v>
       </c>
     </row>
-    <row r="113" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="113" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y113" s="4" t="s">
         <v>112</v>
       </c>
@@ -6671,7 +6610,7 @@
         <v>Bosnia and Herzegovina</v>
       </c>
     </row>
-    <row r="114" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="114" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y114" s="4" t="s">
         <v>113</v>
       </c>
@@ -6697,7 +6636,7 @@
         <v>Bulgaria</v>
       </c>
     </row>
-    <row r="115" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="115" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y115" s="4" t="s">
         <v>114</v>
       </c>
@@ -6723,7 +6662,7 @@
         <v>Croatia</v>
       </c>
     </row>
-    <row r="116" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="116" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y116" s="4" t="s">
         <v>115</v>
       </c>
@@ -6749,7 +6688,7 @@
         <v>Cyprus</v>
       </c>
     </row>
-    <row r="117" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="117" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y117" s="4" t="s">
         <v>116</v>
       </c>
@@ -6775,7 +6714,7 @@
         <v>Czech Republic</v>
       </c>
     </row>
-    <row r="118" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="118" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y118" s="4" t="s">
         <v>117</v>
       </c>
@@ -6801,7 +6740,7 @@
         <v>Denmark</v>
       </c>
     </row>
-    <row r="119" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="119" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y119" s="4" t="s">
         <v>118</v>
       </c>
@@ -6827,7 +6766,7 @@
         <v>Estonia</v>
       </c>
     </row>
-    <row r="120" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="120" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y120" s="4" t="s">
         <v>119</v>
       </c>
@@ -6853,7 +6792,7 @@
         <v>Finland</v>
       </c>
     </row>
-    <row r="121" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="121" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y121" s="4" t="s">
         <v>120</v>
       </c>
@@ -6879,7 +6818,7 @@
         <v>France</v>
       </c>
     </row>
-    <row r="122" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="122" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y122" s="4" t="s">
         <v>121</v>
       </c>
@@ -6905,7 +6844,7 @@
         <v>Georgia</v>
       </c>
     </row>
-    <row r="123" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="123" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y123" s="4" t="s">
         <v>122</v>
       </c>
@@ -6931,7 +6870,7 @@
         <v>Germany</v>
       </c>
     </row>
-    <row r="124" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="124" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y124" s="4" t="s">
         <v>123</v>
       </c>
@@ -6957,7 +6896,7 @@
         <v>Greece</v>
       </c>
     </row>
-    <row r="125" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="125" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y125" s="4" t="s">
         <v>124</v>
       </c>
@@ -6983,7 +6922,7 @@
         <v>Hungary</v>
       </c>
     </row>
-    <row r="126" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="126" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y126" s="4" t="s">
         <v>125</v>
       </c>
@@ -7009,7 +6948,7 @@
         <v>Iceland</v>
       </c>
     </row>
-    <row r="127" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="127" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y127" s="4" t="s">
         <v>126</v>
       </c>
@@ -7035,7 +6974,7 @@
         <v>Ireland</v>
       </c>
     </row>
-    <row r="128" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="128" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y128" s="4" t="s">
         <v>127</v>
       </c>
@@ -7061,7 +7000,7 @@
         <v>Israel</v>
       </c>
     </row>
-    <row r="129" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="129" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y129" s="4" t="s">
         <v>128</v>
       </c>
@@ -7087,7 +7026,7 @@
         <v>Italy</v>
       </c>
     </row>
-    <row r="130" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="130" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y130" s="4" t="s">
         <v>129</v>
       </c>
@@ -7113,7 +7052,7 @@
         <v>Kazakhstan</v>
       </c>
     </row>
-    <row r="131" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="131" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y131" s="4" t="s">
         <v>130</v>
       </c>
@@ -7139,7 +7078,7 @@
         <v>Kyrgyzstan</v>
       </c>
     </row>
-    <row r="132" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="132" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y132" s="4" t="s">
         <v>131</v>
       </c>
@@ -7165,7 +7104,7 @@
         <v>Latvia</v>
       </c>
     </row>
-    <row r="133" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="133" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y133" s="4" t="s">
         <v>132</v>
       </c>
@@ -7191,7 +7130,7 @@
         <v>Lithuania</v>
       </c>
     </row>
-    <row r="134" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="134" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y134" s="4" t="s">
         <v>133</v>
       </c>
@@ -7217,7 +7156,7 @@
         <v>Luxembourg</v>
       </c>
     </row>
-    <row r="135" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="135" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y135" s="4" t="s">
         <v>134</v>
       </c>
@@ -7243,7 +7182,7 @@
         <v>Malta</v>
       </c>
     </row>
-    <row r="136" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="136" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y136" s="4" t="s">
         <v>135</v>
       </c>
@@ -7269,7 +7208,7 @@
         <v>Monaco</v>
       </c>
     </row>
-    <row r="137" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="137" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y137" s="4" t="s">
         <v>136</v>
       </c>
@@ -7295,7 +7234,7 @@
         <v>Montenegro</v>
       </c>
     </row>
-    <row r="138" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="138" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y138" s="4" t="s">
         <v>137</v>
       </c>
@@ -7321,7 +7260,7 @@
         <v>Netherlands</v>
       </c>
     </row>
-    <row r="139" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="139" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y139" s="4" t="s">
         <v>138</v>
       </c>
@@ -7347,7 +7286,7 @@
         <v>Norway</v>
       </c>
     </row>
-    <row r="140" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="140" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y140" s="4" t="s">
         <v>139</v>
       </c>
@@ -7373,7 +7312,7 @@
         <v>Poland</v>
       </c>
     </row>
-    <row r="141" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="141" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y141" s="4" t="s">
         <v>140</v>
       </c>
@@ -7399,7 +7338,7 @@
         <v>Portugal</v>
       </c>
     </row>
-    <row r="142" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="142" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y142" s="4" t="s">
         <v>141</v>
       </c>
@@ -7425,7 +7364,7 @@
         <v>Republic of Moldova</v>
       </c>
     </row>
-    <row r="143" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="143" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y143" s="4" t="s">
         <v>142</v>
       </c>
@@ -7451,7 +7390,7 @@
         <v>Romania</v>
       </c>
     </row>
-    <row r="144" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="144" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y144" s="4" t="s">
         <v>143</v>
       </c>
@@ -7477,7 +7416,7 @@
         <v>Russian Federation</v>
       </c>
     </row>
-    <row r="145" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="145" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y145" s="4" t="s">
         <v>144</v>
       </c>
@@ -7503,7 +7442,7 @@
         <v>San Marino</v>
       </c>
     </row>
-    <row r="146" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="146" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y146" s="4" t="s">
         <v>145</v>
       </c>
@@ -7529,7 +7468,7 @@
         <v>Serbia</v>
       </c>
     </row>
-    <row r="147" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="147" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y147" s="4" t="s">
         <v>146</v>
       </c>
@@ -7555,7 +7494,7 @@
         <v>Slovakia</v>
       </c>
     </row>
-    <row r="148" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="148" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y148" s="4" t="s">
         <v>147</v>
       </c>
@@ -7581,7 +7520,7 @@
         <v>Slovenia</v>
       </c>
     </row>
-    <row r="149" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="149" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y149" s="4" t="s">
         <v>148</v>
       </c>
@@ -7607,7 +7546,7 @@
         <v>Spain</v>
       </c>
     </row>
-    <row r="150" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="150" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y150" s="4" t="s">
         <v>149</v>
       </c>
@@ -7633,7 +7572,7 @@
         <v>Sweden</v>
       </c>
     </row>
-    <row r="151" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="151" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y151" s="4" t="s">
         <v>150</v>
       </c>
@@ -7659,7 +7598,7 @@
         <v>Switzerland</v>
       </c>
     </row>
-    <row r="152" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="152" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y152" s="4" t="s">
         <v>151</v>
       </c>
@@ -7685,7 +7624,7 @@
         <v>Tajikistan</v>
       </c>
     </row>
-    <row r="153" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="153" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y153" s="4" t="s">
         <v>152</v>
       </c>
@@ -7711,7 +7650,7 @@
         <v>The former Yugoslav republic of Macedonia</v>
       </c>
     </row>
-    <row r="154" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="154" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y154" s="4" t="s">
         <v>153</v>
       </c>
@@ -7737,7 +7676,7 @@
         <v>Turkey</v>
       </c>
     </row>
-    <row r="155" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="155" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y155" s="4" t="s">
         <v>511</v>
       </c>
@@ -7763,7 +7702,7 @@
         <v>Turkmenistan</v>
       </c>
     </row>
-    <row r="156" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="156" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y156" s="4" t="s">
         <v>154</v>
       </c>
@@ -7789,7 +7728,7 @@
         <v>Ukraine</v>
       </c>
     </row>
-    <row r="157" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="157" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y157" s="4" t="s">
         <v>155</v>
       </c>
@@ -7815,7 +7754,7 @@
         <v>United Kingdom of Great Britain and Northern Ireland</v>
       </c>
     </row>
-    <row r="158" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="158" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y158" s="4" t="s">
         <v>156</v>
       </c>
@@ -7841,7 +7780,7 @@
         <v>Uzbekistan</v>
       </c>
     </row>
-    <row r="159" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="159" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y159" s="4" t="s">
         <v>520</v>
       </c>
@@ -7867,7 +7806,7 @@
         <v>American Samoa</v>
       </c>
     </row>
-    <row r="160" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="160" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y160" s="4" t="s">
         <v>157</v>
       </c>
@@ -7893,7 +7832,7 @@
         <v>Anguilla</v>
       </c>
     </row>
-    <row r="161" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="161" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y161" s="4" t="s">
         <v>525</v>
       </c>
@@ -7919,7 +7858,7 @@
         <v>Aruba</v>
       </c>
     </row>
-    <row r="162" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="162" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y162" s="4" t="s">
         <v>529</v>
       </c>
@@ -7945,7 +7884,7 @@
         <v>Bermuda</v>
       </c>
     </row>
-    <row r="163" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="163" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y163" s="4" t="s">
         <v>532</v>
       </c>
@@ -7971,7 +7910,7 @@
         <v>Bonaire, Saint Eustatius and Saba</v>
       </c>
     </row>
-    <row r="164" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="164" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y164" s="4" t="s">
         <v>535</v>
       </c>
@@ -7997,7 +7936,7 @@
         <v>British Virgin Islands</v>
       </c>
     </row>
-    <row r="165" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="165" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y165" s="4" t="s">
         <v>538</v>
       </c>
@@ -8023,7 +7962,7 @@
         <v>Cayman Islands</v>
       </c>
     </row>
-    <row r="166" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="166" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y166" s="4" t="s">
         <v>541</v>
       </c>
@@ -8049,7 +7988,7 @@
         <v>China, Hong Kong Special Administrative Region</v>
       </c>
     </row>
-    <row r="167" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="167" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y167" s="4" t="s">
         <v>544</v>
       </c>
@@ -8075,7 +8014,7 @@
         <v>China, Macao Special Administrative Region</v>
       </c>
     </row>
-    <row r="168" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="168" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y168" s="4" t="s">
         <v>547</v>
       </c>
@@ -8101,7 +8040,7 @@
         <v>China: Province of Taiwan only</v>
       </c>
     </row>
-    <row r="169" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="169" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y169" s="4" t="s">
         <v>550</v>
       </c>
@@ -8127,7 +8066,7 @@
         <v>Curacao</v>
       </c>
     </row>
-    <row r="170" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="170" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y170" s="4" t="s">
         <v>553</v>
       </c>
@@ -8153,7 +8092,7 @@
         <v>Czechoslovakia, Former</v>
       </c>
     </row>
-    <row r="171" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="171" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y171" s="4" t="s">
         <v>556</v>
       </c>
@@ -8179,7 +8118,7 @@
         <v>Falkland Islands (Malvinas)</v>
       </c>
     </row>
-    <row r="172" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="172" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y172" s="4" t="s">
         <v>559</v>
       </c>
@@ -8205,7 +8144,7 @@
         <v>Faroe Islands</v>
       </c>
     </row>
-    <row r="173" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="173" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y173" s="4" t="s">
         <v>562</v>
       </c>
@@ -8231,7 +8170,7 @@
         <v>French Guiana</v>
       </c>
     </row>
-    <row r="174" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="174" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y174" s="4" t="s">
         <v>565</v>
       </c>
@@ -8257,7 +8196,7 @@
         <v>French Polynesia</v>
       </c>
     </row>
-    <row r="175" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="175" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y175" s="4" t="s">
         <v>568</v>
       </c>
@@ -8283,7 +8222,7 @@
         <v>Germany, Former Democratic Republic</v>
       </c>
     </row>
-    <row r="176" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="176" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y176" s="4" t="s">
         <v>571</v>
       </c>
@@ -8309,7 +8248,7 @@
         <v>Germany, Former Federal Republic</v>
       </c>
     </row>
-    <row r="177" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="177" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y177" s="4" t="s">
         <v>574</v>
       </c>
@@ -8335,7 +8274,7 @@
         <v>Germany, West Berlin</v>
       </c>
     </row>
-    <row r="178" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="178" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y178" s="4" t="s">
         <v>577</v>
       </c>
@@ -8361,7 +8300,7 @@
         <v>Gibraltar</v>
       </c>
     </row>
-    <row r="179" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="179" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y179" s="4" t="s">
         <v>580</v>
       </c>
@@ -8387,7 +8326,7 @@
         <v>Greenland</v>
       </c>
     </row>
-    <row r="180" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="180" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y180" s="4" t="s">
         <v>583</v>
       </c>
@@ -8413,7 +8352,7 @@
         <v>Guadeloupe</v>
       </c>
     </row>
-    <row r="181" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="181" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y181" s="4" t="s">
         <v>586</v>
       </c>
@@ -8439,7 +8378,7 @@
         <v>Guam</v>
       </c>
     </row>
-    <row r="182" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="182" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y182" s="4" t="s">
         <v>589</v>
       </c>
@@ -8465,7 +8404,7 @@
         <v>Liechtenstein</v>
       </c>
     </row>
-    <row r="183" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="183" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y183" s="4" t="s">
         <v>592</v>
       </c>
@@ -8491,7 +8430,7 @@
         <v>Martinique</v>
       </c>
     </row>
-    <row r="184" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="184" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y184" s="4" t="s">
         <v>595</v>
       </c>
@@ -8517,7 +8456,7 @@
         <v>Mayotte</v>
       </c>
     </row>
-    <row r="185" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="185" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y185" s="4" t="s">
         <v>598</v>
       </c>
@@ -8543,7 +8482,7 @@
         <v>Montserrat</v>
       </c>
     </row>
-    <row r="186" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="186" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y186" s="4" t="s">
         <v>601</v>
       </c>
@@ -8569,7 +8508,7 @@
         <v>Netherlands Antilles</v>
       </c>
     </row>
-    <row r="187" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="187" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y187" s="4" t="s">
         <v>604</v>
       </c>
@@ -8595,7 +8534,7 @@
         <v>New Caledonia</v>
       </c>
     </row>
-    <row r="188" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="188" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y188" s="4" t="s">
         <v>607</v>
       </c>
@@ -8621,7 +8560,7 @@
         <v>Norfolk Island</v>
       </c>
     </row>
-    <row r="189" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="189" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y189" s="4" t="s">
         <v>610</v>
       </c>
@@ -8647,7 +8586,7 @@
         <v>Northern Mariana Islands</v>
       </c>
     </row>
-    <row r="190" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="190" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y190" s="4" t="s">
         <v>613</v>
       </c>
@@ -8673,7 +8612,7 @@
         <v>Pitcairn Island</v>
       </c>
     </row>
-    <row r="191" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="191" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y191" s="4" t="s">
         <v>616</v>
       </c>
@@ -8699,7 +8638,7 @@
         <v>Puerto Rico</v>
       </c>
     </row>
-    <row r="192" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="192" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y192" s="4" t="s">
         <v>619</v>
       </c>
@@ -8725,7 +8664,7 @@
         <v>Rodrigues</v>
       </c>
     </row>
-    <row r="193" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="193" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y193" s="4" t="s">
         <v>622</v>
       </c>
@@ -8751,7 +8690,7 @@
         <v>Rï¿½union</v>
       </c>
     </row>
-    <row r="194" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="194" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y194" s="4" t="s">
         <v>625</v>
       </c>
@@ -8777,7 +8716,7 @@
         <v>Ryu Kyu Islands</v>
       </c>
     </row>
-    <row r="195" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="195" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y195" s="4" t="s">
         <v>628</v>
       </c>
@@ -8803,7 +8742,7 @@
         <v>Saint Helena</v>
       </c>
     </row>
-    <row r="196" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="196" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y196" s="4" t="s">
         <v>631</v>
       </c>
@@ -8829,7 +8768,7 @@
         <v>Saint Pierre and Miquelon</v>
       </c>
     </row>
-    <row r="197" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="197" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y197" s="4" t="s">
         <v>634</v>
       </c>
@@ -8855,7 +8794,7 @@
         <v>Serbia and Montenegro, Former</v>
       </c>
     </row>
-    <row r="198" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="198" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y198" s="4" t="s">
         <v>637</v>
       </c>
@@ -8881,7 +8820,7 @@
         <v>Sint Maarten (Dutch part)</v>
       </c>
     </row>
-    <row r="199" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="199" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y199" s="4" t="s">
         <v>640</v>
       </c>
@@ -8907,7 +8846,7 @@
         <v>Sudan (former)</v>
       </c>
     </row>
-    <row r="200" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="200" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y200" s="4" t="s">
         <v>643</v>
       </c>
@@ -8933,7 +8872,7 @@
         <v>The former state union Serbia and Montenegro</v>
       </c>
     </row>
-    <row r="201" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="201" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y201" s="4" t="s">
         <v>646</v>
       </c>
@@ -8959,7 +8898,7 @@
         <v>Tokelau</v>
       </c>
     </row>
-    <row r="202" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="202" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y202" s="4" t="s">
         <v>649</v>
       </c>
@@ -8985,7 +8924,7 @@
         <v>Turks and Caicos Islands</v>
       </c>
     </row>
-    <row r="203" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="203" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y203" s="4" t="s">
         <v>652</v>
       </c>
@@ -9011,7 +8950,7 @@
         <v>United Kingdom, England and Wales</v>
       </c>
     </row>
-    <row r="204" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="204" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y204" s="4" t="s">
         <v>655</v>
       </c>
@@ -9037,7 +8976,7 @@
         <v>United Kingdom, Northern Ireland</v>
       </c>
     </row>
-    <row r="205" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="205" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y205" s="4" t="s">
         <v>658</v>
       </c>
@@ -9063,7 +9002,7 @@
         <v>United Kingdom, Scotland</v>
       </c>
     </row>
-    <row r="206" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="206" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y206" s="4" t="s">
         <v>661</v>
       </c>
@@ -9089,7 +9028,7 @@
         <v>USSR, Former</v>
       </c>
     </row>
-    <row r="207" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="207" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y207" s="4" t="s">
         <v>664</v>
       </c>
@@ -9115,7 +9054,7 @@
         <v>Virgin Islands (USA)</v>
       </c>
     </row>
-    <row r="208" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="208" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y208" s="4" t="s">
         <v>667</v>
       </c>
@@ -9141,7 +9080,7 @@
         <v>Wallis and Futuna Islands</v>
       </c>
     </row>
-    <row r="209" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="209" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y209" s="4" t="s">
         <v>670</v>
       </c>
@@ -9167,7 +9106,7 @@
         <v>West Bank</v>
       </c>
     </row>
-    <row r="210" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="210" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y210" s="4" t="s">
         <v>673</v>
       </c>
@@ -9193,7 +9132,7 @@
         <v>Yugoslavia, Former</v>
       </c>
     </row>
-    <row r="211" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="211" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y211" s="4" t="s">
         <v>676</v>
       </c>
@@ -9219,7 +9158,7 @@
         <v>Bangladesh</v>
       </c>
     </row>
-    <row r="212" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="212" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y212" s="4" t="s">
         <v>679</v>
       </c>
@@ -9245,7 +9184,7 @@
         <v>Bhutan</v>
       </c>
     </row>
-    <row r="213" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="213" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y213" s="4" t="s">
         <v>158</v>
       </c>
@@ -9271,7 +9210,7 @@
         <v>Democratic People's Republic of Korea</v>
       </c>
     </row>
-    <row r="214" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="214" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y214" s="4" t="s">
         <v>159</v>
       </c>
@@ -9297,7 +9236,7 @@
         <v>India</v>
       </c>
     </row>
-    <row r="215" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="215" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y215" s="4" t="s">
         <v>160</v>
       </c>
@@ -9323,7 +9262,7 @@
         <v>Indonesia</v>
       </c>
     </row>
-    <row r="216" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="216" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y216" s="4" t="s">
         <v>161</v>
       </c>
@@ -9349,7 +9288,7 @@
         <v>Maldives</v>
       </c>
     </row>
-    <row r="217" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="217" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y217" s="4" t="s">
         <v>162</v>
       </c>
@@ -9375,7 +9314,7 @@
         <v>Myanmar</v>
       </c>
     </row>
-    <row r="218" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="218" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y218" s="4" t="s">
         <v>163</v>
       </c>
@@ -9401,7 +9340,7 @@
         <v>Nepal</v>
       </c>
     </row>
-    <row r="219" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="219" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y219" s="4" t="s">
         <v>164</v>
       </c>
@@ -9427,7 +9366,7 @@
         <v>Sri Lanka</v>
       </c>
     </row>
-    <row r="220" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="220" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y220" s="4" t="s">
         <v>165</v>
       </c>
@@ -9453,7 +9392,7 @@
         <v>Thailand</v>
       </c>
     </row>
-    <row r="221" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="221" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y221" s="4" t="s">
         <v>166</v>
       </c>
@@ -9479,7 +9418,7 @@
         <v>Timor-Leste</v>
       </c>
     </row>
-    <row r="222" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="222" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y222" s="4" t="s">
         <v>167</v>
       </c>
@@ -9505,7 +9444,7 @@
         <v>Australia</v>
       </c>
     </row>
-    <row r="223" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="223" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y223" s="4" t="s">
         <v>168</v>
       </c>
@@ -9531,7 +9470,7 @@
         <v>Brunei Darussalam</v>
       </c>
     </row>
-    <row r="224" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="224" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y224" s="4" t="s">
         <v>169</v>
       </c>
@@ -9557,7 +9496,7 @@
         <v>Cambodia</v>
       </c>
     </row>
-    <row r="225" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="225" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y225" s="4" t="s">
         <v>170</v>
       </c>
@@ -9583,7 +9522,7 @@
         <v>China</v>
       </c>
     </row>
-    <row r="226" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="226" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y226" s="4" t="s">
         <v>171</v>
       </c>
@@ -9609,7 +9548,7 @@
         <v>Cook Islands</v>
       </c>
     </row>
-    <row r="227" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="227" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y227" s="4" t="s">
         <v>712</v>
       </c>
@@ -9635,7 +9574,7 @@
         <v>Fiji</v>
       </c>
     </row>
-    <row r="228" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="228" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y228" s="4" t="s">
         <v>172</v>
       </c>
@@ -9661,7 +9600,7 @@
         <v>Japan</v>
       </c>
     </row>
-    <row r="229" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="229" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y229" s="4" t="s">
         <v>173</v>
       </c>
@@ -9687,7 +9626,7 @@
         <v>Kiribati</v>
       </c>
     </row>
-    <row r="230" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="230" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y230" s="4" t="s">
         <v>174</v>
       </c>
@@ -9713,7 +9652,7 @@
         <v>Lao People's Democratic Republic</v>
       </c>
     </row>
-    <row r="231" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="231" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y231" s="4" t="s">
         <v>175</v>
       </c>
@@ -9739,7 +9678,7 @@
         <v>Malaysia</v>
       </c>
     </row>
-    <row r="232" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="232" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y232" s="4" t="s">
         <v>176</v>
       </c>
@@ -9765,7 +9704,7 @@
         <v>Marshall Islands</v>
       </c>
     </row>
-    <row r="233" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="233" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y233" s="4" t="s">
         <v>177</v>
       </c>
@@ -9791,7 +9730,7 @@
         <v>Micronesia (Federated States of)</v>
       </c>
     </row>
-    <row r="234" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="234" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y234" s="4" t="s">
         <v>178</v>
       </c>
@@ -9817,7 +9756,7 @@
         <v>Mongolia</v>
       </c>
     </row>
-    <row r="235" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="235" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y235" s="4" t="s">
         <v>179</v>
       </c>
@@ -9843,7 +9782,7 @@
         <v>Nauru</v>
       </c>
     </row>
-    <row r="236" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="236" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y236" s="4" t="s">
         <v>180</v>
       </c>
@@ -9869,7 +9808,7 @@
         <v>New Zealand</v>
       </c>
     </row>
-    <row r="237" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="237" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y237" s="4" t="s">
         <v>181</v>
       </c>
@@ -9895,7 +9834,7 @@
         <v>Niue</v>
       </c>
     </row>
-    <row r="238" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="238" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y238" s="4" t="s">
         <v>182</v>
       </c>
@@ -9921,7 +9860,7 @@
         <v>Palau</v>
       </c>
     </row>
-    <row r="239" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="239" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y239" s="4" t="s">
         <v>183</v>
       </c>
@@ -9947,7 +9886,7 @@
         <v>Papua New Guinea</v>
       </c>
     </row>
-    <row r="240" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="240" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y240" s="4" t="s">
         <v>739</v>
       </c>
@@ -9973,7 +9912,7 @@
         <v>Philippines</v>
       </c>
     </row>
-    <row r="241" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="241" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y241" s="4" t="s">
         <v>184</v>
       </c>
@@ -9999,7 +9938,7 @@
         <v>Republic of Korea</v>
       </c>
     </row>
-    <row r="242" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="242" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y242" s="4" t="s">
         <v>185</v>
       </c>
@@ -10025,7 +9964,7 @@
         <v>Samoa</v>
       </c>
     </row>
-    <row r="243" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="243" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y243" s="4" t="s">
         <v>186</v>
       </c>
@@ -10051,7 +9990,7 @@
         <v>Singapore</v>
       </c>
     </row>
-    <row r="244" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="244" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y244" s="4" t="s">
         <v>187</v>
       </c>
@@ -10077,7 +10016,7 @@
         <v>Solomon Islands</v>
       </c>
     </row>
-    <row r="245" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="245" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y245" s="4" t="s">
         <v>188</v>
       </c>
@@ -10103,7 +10042,7 @@
         <v>Tonga</v>
       </c>
     </row>
-    <row r="246" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="246" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y246" s="4" t="s">
         <v>189</v>
       </c>
@@ -10129,7 +10068,7 @@
         <v>Tuvalu</v>
       </c>
     </row>
-    <row r="247" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="247" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y247" s="4" t="s">
         <v>190</v>
       </c>
@@ -10155,7 +10094,7 @@
         <v>Vanuatu</v>
       </c>
     </row>
-    <row r="248" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="248" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y248" s="4" t="s">
         <v>191</v>
       </c>
@@ -10181,7 +10120,7 @@
         <v>Viet Nam</v>
       </c>
     </row>
-    <row r="249" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="249" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y249" s="4" t="s">
         <v>192</v>
       </c>
@@ -10207,7 +10146,7 @@
         <v/>
       </c>
     </row>
-    <row r="250" spans="25:31" x14ac:dyDescent="0.4">
+    <row r="250" spans="25:31" x14ac:dyDescent="0.25">
       <c r="Y250" s="4" t="s">
         <v>193</v>
       </c>
@@ -10234,8 +10173,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="kkgcrUNc5enmSCaWgQb/8MKXVL+Xe/lDbLJNN54ML8xg/f+fgIaEPY7w/CMhXz+P5L4TgQMkXLTtXwn3Cpd75g==" saltValue="YNiqkgimZRwsNwEU0zK5Mg==" spinCount="100000" sheet="1" selectLockedCells="1"/>
-  <mergeCells count="14">
+  <sheetProtection algorithmName="SHA-512" hashValue="PVDL0C1ysPyvWA5e+0rjI6WUHRbz3jaHsApeSGUpku0WVpZeOLEtOOrXMXY62jl3D8S4fAEOzSS0l53A6vktqg==" saltValue="R9x8HS/3Pu2LodJa2YD6sQ==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <mergeCells count="13">
     <mergeCell ref="B1:I1"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="E7:G7"/>
@@ -10249,13 +10188,12 @@
     <mergeCell ref="F15:G15"/>
     <mergeCell ref="D13:E14"/>
     <mergeCell ref="F13:G14"/>
-    <mergeCell ref="B11:G12"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:G10">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:G10" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>YEAR(TODAY())-20</formula1>
       <formula2>YEAR(TODAY())-1</formula2>
     </dataValidation>
@@ -10272,13 +10210,13 @@
             <anchor moveWithCells="1" sizeWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>713014</xdr:colOff>
+                <xdr:colOff>714375</xdr:colOff>
                 <xdr:row>2</xdr:row>
-                <xdr:rowOff>277586</xdr:rowOff>
+                <xdr:rowOff>276225</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>10886</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>38100</xdr:rowOff>
               </to>
@@ -10297,15 +10235,15 @@
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>620486</xdr:colOff>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>14</xdr:row>
-                <xdr:rowOff>179614</xdr:rowOff>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>963386</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>478971</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>15</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
@@ -10317,7 +10255,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:N15"/>
   <sheetViews>
@@ -10325,63 +10263,63 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.15234375" style="4"/>
-    <col min="2" max="2" width="10.84375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="53.3828125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="22.15234375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="22.3046875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="4" customWidth="1"/>
     <col min="6" max="6" width="22" style="4" customWidth="1"/>
     <col min="7" max="7" width="24" style="4" customWidth="1"/>
-    <col min="8" max="8" width="18.3828125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="9.69140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="4" customWidth="1"/>
     <col min="10" max="10" width="10" style="4" customWidth="1"/>
-    <col min="11" max="11" width="11.53515625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="9.84375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="8.84375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="9.15234375" style="4" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="4" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.15234375" style="4"/>
+    <col min="16" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="22.75" x14ac:dyDescent="0.4">
-      <c r="B1" s="44" t="s">
+    <row r="1" spans="2:14" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-    </row>
-    <row r="2" spans="2:14" ht="22.75" x14ac:dyDescent="0.4">
-      <c r="B2" s="44" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+    </row>
+    <row r="2" spans="2:14" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B2" s="39" t="s">
         <v>770</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
       <c r="N2" s="11" t="e">
         <f>Finance!V2</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="22.75" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:14" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
@@ -10396,160 +10334,160 @@
       <c r="M3" s="18"/>
       <c r="N3" s="11"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B4" s="33" t="s">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="35" t="str">
+      <c r="C4" s="32" t="str">
         <f>Finance!V1</f>
         <v/>
       </c>
-      <c r="E4" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="35" t="str">
+      <c r="E4" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="32" t="str">
         <f>Finance!F4</f>
         <v/>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="32">
         <f>Finance!I4</f>
         <v>0</v>
       </c>
       <c r="N4" s="11"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="L5" s="5"/>
       <c r="N5" s="11"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L6" s="5"/>
       <c r="N6" s="11"/>
     </row>
-    <row r="7" spans="2:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="57" t="s">
+    <row r="7" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="C7" s="45" t="s">
         <v>783</v>
       </c>
-      <c r="D7" s="55" t="s">
+      <c r="D7" s="42" t="s">
         <v>776</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="42" t="s">
         <v>777</v>
       </c>
-      <c r="F7" s="55" t="s">
+      <c r="F7" s="42" t="s">
         <v>778</v>
       </c>
-      <c r="G7" s="54" t="s">
+      <c r="G7" s="41" t="s">
         <v>779</v>
       </c>
       <c r="N7" s="11"/>
     </row>
-    <row r="8" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="57"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="54"/>
+    <row r="8" spans="2:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="44"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="41"/>
       <c r="N8" s="11"/>
     </row>
-    <row r="9" spans="2:14" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
       <c r="N9" s="11" t="str">
         <f>IF(N8=2,"true",IF(N8=3,"false",""))</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>2</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>792</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
       <c r="N10" s="11"/>
     </row>
-    <row r="11" spans="2:14" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>3</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>793</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-    </row>
-    <row r="12" spans="2:14" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+    </row>
+    <row r="12" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>4</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-    </row>
-    <row r="13" spans="2:14" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+    </row>
+    <row r="13" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>5</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-    </row>
-    <row r="14" spans="2:14" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+    </row>
+    <row r="14" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>6</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-    </row>
-    <row r="15" spans="2:14" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+    </row>
+    <row r="15" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
         <v>7</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="10+Rrl0ghWqtWia3R2g7RY0L2rG8GfvF8KX3JHyfPtNS3WJs6nRw1QdBKjS6h3OZ+nCgT4fdLEdlsj+0sNeYqg==" saltValue="nhUBTdv5HVUaCq9sqcQ1kQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="QdWhi2T7aJ2us9B+XDDC/wHfWcwC1MY+KorLLctEYSysZ49jy1vAErCtnTbVrOVAZgvOmAVkZcLjt9og3qA3tw==" saltValue="zte0L/aMCCb9Qr9XhIisyA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="8">
     <mergeCell ref="G7:G8"/>
     <mergeCell ref="F7:F8"/>
@@ -10561,7 +10499,7 @@
     <mergeCell ref="E7:E8"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:G15">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:G15" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -10571,7 +10509,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:Q51"/>
   <sheetViews>
@@ -10579,33 +10517,33 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.53515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="15" style="4" customWidth="1"/>
-    <col min="3" max="3" width="40.69140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="40.3046875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="24.3828125" style="4" customWidth="1"/>
-    <col min="6" max="8" width="20.69140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="18.53515625" style="4" customWidth="1"/>
-    <col min="10" max="12" width="16.3828125" style="4" customWidth="1"/>
-    <col min="13" max="14" width="18.3046875" style="4" customWidth="1"/>
-    <col min="15" max="15" width="16.3828125" style="4" customWidth="1"/>
-    <col min="16" max="17" width="9.15234375" style="4" hidden="1" customWidth="1"/>
-    <col min="18" max="43" width="9.15234375" style="4" customWidth="1"/>
-    <col min="44" max="16384" width="9.15234375" style="4"/>
+    <col min="1" max="1" width="9.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" style="4" customWidth="1"/>
+    <col min="6" max="8" width="20.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" style="4" customWidth="1"/>
+    <col min="10" max="12" width="16.42578125" style="4" customWidth="1"/>
+    <col min="13" max="14" width="18.28515625" style="4" customWidth="1"/>
+    <col min="15" max="15" width="16.42578125" style="4" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="4" hidden="1" customWidth="1"/>
+    <col min="18" max="43" width="9.140625" style="4" customWidth="1"/>
+    <col min="44" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="22.75" x14ac:dyDescent="0.4">
-      <c r="B1" s="44" t="s">
+    <row r="1" spans="2:16" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -10614,16 +10552,16 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="2:16" ht="22.75" x14ac:dyDescent="0.4">
-      <c r="B2" s="44" t="s">
+    <row r="2" spans="2:16" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B2" s="39" t="s">
         <v>771</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -10636,48 +10574,48 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="2:16" ht="22.75" x14ac:dyDescent="0.4">
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-    </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B4" s="33" t="s">
+    <row r="3" spans="2:16" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="35" t="str">
+      <c r="C4" s="32" t="str">
         <f>Finance!V1</f>
         <v/>
       </c>
-      <c r="E4" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="35" t="str">
+      <c r="E4" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="32" t="str">
         <f>Finance!F4</f>
         <v/>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="32">
         <f>Finance!I4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="22.75" x14ac:dyDescent="0.4">
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+    <row r="5" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -10691,22 +10629,22 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="2:16" ht="39" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="57" t="s">
+    <row r="6" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="41" t="s">
         <v>782</v>
       </c>
-      <c r="D6" s="55" t="s">
+      <c r="D6" s="42" t="s">
         <v>784</v>
       </c>
-      <c r="E6" s="54" t="s">
-        <v>784</v>
-      </c>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
+      <c r="E6" s="41" t="s">
+        <v>801</v>
+      </c>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
       <c r="I6" s="19"/>
       <c r="J6" s="19"/>
       <c r="K6" s="19"/>
@@ -10715,18 +10653,18 @@
       <c r="N6" s="19"/>
       <c r="O6" s="19"/>
     </row>
-    <row r="7" spans="2:16" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="57"/>
-      <c r="C7" s="57"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="54" t="s">
+    <row r="7" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="41" t="s">
         <v>766</v>
       </c>
-      <c r="F7" s="61" t="s">
+      <c r="F7" s="48" t="s">
         <v>762</v>
       </c>
-      <c r="G7" s="54"/>
-      <c r="H7" s="54"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
       <c r="I7" s="19"/>
       <c r="J7" s="19"/>
       <c r="K7" s="19"/>
@@ -10735,33 +10673,33 @@
       <c r="N7" s="19"/>
       <c r="O7" s="19"/>
     </row>
-    <row r="8" spans="2:16" ht="51.45" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="57"/>
-      <c r="C8" s="57"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="30" t="s">
+    <row r="8" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="27" t="s">
         <v>785</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="27" t="s">
         <v>786</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="28" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>1</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>794</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
       <c r="K9" s="19"/>
@@ -10769,18 +10707,18 @@
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
     </row>
-    <row r="10" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>2</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>780</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="19"/>
@@ -10789,18 +10727,18 @@
       <c r="N10" s="19"/>
       <c r="O10" s="19"/>
     </row>
-    <row r="11" spans="2:16" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>3</v>
       </c>
       <c r="C11" s="17" t="s">
         <v>795</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="57"/>
       <c r="I11" s="19"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
@@ -10809,18 +10747,18 @@
       <c r="N11" s="19"/>
       <c r="O11" s="19"/>
     </row>
-    <row r="12" spans="2:16" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>4</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>781</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
       <c r="I12" s="19"/>
       <c r="J12" s="19"/>
       <c r="K12" s="19"/>
@@ -10829,18 +10767,18 @@
       <c r="N12" s="19"/>
       <c r="O12" s="19"/>
     </row>
-    <row r="13" spans="2:16" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>5</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>796</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
       <c r="I13" s="19"/>
       <c r="J13" s="19"/>
       <c r="K13" s="19"/>
@@ -10849,18 +10787,18 @@
       <c r="N13" s="19"/>
       <c r="O13" s="19"/>
     </row>
-    <row r="14" spans="2:16" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>6</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>797</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+      <c r="H14" s="57"/>
       <c r="I14" s="19"/>
       <c r="J14" s="19"/>
       <c r="K14" s="19"/>
@@ -10869,7 +10807,7 @@
       <c r="N14" s="19"/>
       <c r="O14" s="19"/>
     </row>
-    <row r="15" spans="2:16" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
       <c r="D15" s="19"/>
@@ -10885,46 +10823,46 @@
       <c r="N15" s="19"/>
       <c r="O15" s="19"/>
     </row>
-    <row r="16" spans="2:16" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="17" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="E17" s="28"/>
-    </row>
-    <row r="18" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="19" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="20" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="21" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="22" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="23" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="24" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="25" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="26" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="27" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="28" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="29" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="30" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="31" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="32" spans="5:5" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="33" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="34" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="35" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="36" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="37" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="38" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="39" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="40" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="41" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="42" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="43" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="44" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="45" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="46" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="47" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="48" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="49" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="50" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="51" ht="14.7" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="16" spans="2:16" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="25"/>
+    </row>
+    <row r="18" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="5:5" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="14.65" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="pbnRlw/nYjj+kULKnscvcBVhseTBWKFuTsJ8jRQidx70ncdZtcbmlc1d8UGefKd2P/2T2mNrzY7A4pcCbEcG9A==" saltValue="HOROEzEUHXoWgqC7C4Hm4w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="U7k+usCdgMph2iOW6ga3ej3AHiy7ljvHvNwcldwyh1PqwkKEjSd/s6EQC/K8ksAz+apfREzBLtKMaSIKZNSVxw==" saltValue="LOo6jCoiN/9ni4RGD+jhOQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="8">
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B2:H2"/>
@@ -10936,7 +10874,7 @@
     <mergeCell ref="E7:E8"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:H14">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:H14" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -10946,251 +10884,251 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:N17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.15234375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.15234375" style="4"/>
-    <col min="2" max="2" width="10.84375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="53.3828125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="20.3828125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="22.3046875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="29.84375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="10.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="23" style="4" customWidth="1"/>
-    <col min="8" max="8" width="18.3828125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="9.69140625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="4" customWidth="1"/>
     <col min="10" max="10" width="10" style="4" customWidth="1"/>
-    <col min="11" max="11" width="11.53515625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="9.84375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="8.84375" style="4" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="9.15234375" style="4" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="4" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="4" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="4" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="0" style="4" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.15234375" style="4"/>
+    <col min="16" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="22.75" x14ac:dyDescent="0.4">
-      <c r="B1" s="44" t="s">
+    <row r="1" spans="2:14" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-    </row>
-    <row r="2" spans="2:14" ht="22.75" x14ac:dyDescent="0.4">
-      <c r="B2" s="44" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+    </row>
+    <row r="2" spans="2:14" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B2" s="39" t="s">
         <v>770</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
       <c r="N2" s="4" t="e">
         <f>Finance!V2</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="22.75" x14ac:dyDescent="0.4">
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B4" s="33" t="s">
+    <row r="3" spans="2:14" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="35" t="str">
+      <c r="C4" s="32" t="str">
         <f>Finance!V1</f>
         <v/>
       </c>
-      <c r="E4" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="35" t="str">
+      <c r="E4" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="32" t="str">
         <f>Finance!F4</f>
         <v/>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="32">
         <f>Finance!I4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="2:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="71" t="s">
+    <row r="7" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="44" t="s">
         <v>783</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="41" t="s">
         <v>788</v>
       </c>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="64"/>
-    </row>
-    <row r="8" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="G8" s="67"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="58" t="s">
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+    </row>
+    <row r="8" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+    </row>
+    <row r="9" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44" t="s">
         <v>766</v>
       </c>
-      <c r="E9" s="68" t="s">
+      <c r="E9" s="44" t="s">
         <v>762</v>
       </c>
-      <c r="F9" s="69"/>
-      <c r="G9" s="70"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
       <c r="N9" s="4" t="str">
         <f>IF(N8=2,"true",IF(N8=3,"false",""))</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="2:14" ht="27" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="31" t="s">
+    <row r="10" spans="2:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="36" t="s">
         <v>767</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="36" t="s">
         <v>789</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="36" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="15.9" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-    </row>
-    <row r="12" spans="2:14" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D11" s="57"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="57"/>
+    </row>
+    <row r="12" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>2</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>792</v>
       </c>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-    </row>
-    <row r="13" spans="2:14" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="57"/>
+    </row>
+    <row r="13" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>3</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>793</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-    </row>
-    <row r="14" spans="2:14" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+    </row>
+    <row r="14" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>4</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-    </row>
-    <row r="15" spans="2:14" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D14" s="57"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="57"/>
+    </row>
+    <row r="15" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
         <v>5</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-    </row>
-    <row r="16" spans="2:14" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D15" s="57"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="57"/>
+    </row>
+    <row r="16" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="6">
         <v>6</v>
       </c>
       <c r="C16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-    </row>
-    <row r="17" spans="2:7" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="D16" s="57"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="57"/>
+    </row>
+    <row r="17" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
         <v>7</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="57"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="h1oGcdmgRfQcZlr9KawMFlUKqYgu1fXyHEqtnhKmhRM8ybMI/C/5zPhZ941qmV9HA3Z9TXxhvLi+EKfykKYsmA==" saltValue="vkM8tazx6gjKqf5VXQwDfw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="T6A1oqgEmONkUzRDjMX80FZoQYLKyL7mNekzPQ124Y8FVXQZYtsVBPz/vKqu761J4RpD4ho/xFCjTpf61lQzZg==" saltValue="KfMTOmCXgmd2Tf3RebmQyg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="7">
     <mergeCell ref="D7:G8"/>
     <mergeCell ref="D9:D10"/>
@@ -11201,7 +11139,7 @@
     <mergeCell ref="C7:C10"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:G17">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D11:G17" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>